<commit_message>
ajustando simbolos de setas
</commit_message>
<xml_diff>
--- a/_data/store-data.xlsx
+++ b/_data/store-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Desktop\ProjetoCheatSheets\cheatsheets\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10398DD-9A3C-41D2-86A1-78DDD72E295A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F463934-AFB9-4C77-B3A7-FE032474AA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="405" yWindow="360" windowWidth="27615" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="store-data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="318">
   <si>
     <t>comandos</t>
   </si>
@@ -985,6 +985,9 @@
   </si>
   <si>
     <t>grade2</t>
+  </si>
+  <si>
+    <t>Ctrl+ &amp;#9650; / &amp;#9660;</t>
   </si>
 </sst>
 </file>
@@ -1831,8 +1834,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D148" sqref="D148:D150"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4346,7 +4349,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>105</v>
+        <v>317</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>298</v>

</xml_diff>

<commit_message>
arrumando simbolos de setas
</commit_message>
<xml_diff>
--- a/_data/store-data.xlsx
+++ b/_data/store-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Desktop\ProjetoCheatSheets\cheatsheets\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F463934-AFB9-4C77-B3A7-FE032474AA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B140DE-4C6C-49D8-89BD-3E3A653DB88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="405" yWindow="360" windowWidth="27615" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -294,15 +294,9 @@
     <t xml:space="preserve"> Copy line (empty selection)</t>
   </si>
   <si>
-    <t>Alt+ ↑ / ↓</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Move line up/down</t>
   </si>
   <si>
-    <t>Shift+Alt + ↓ / ↑</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Copy line up/down</t>
   </si>
   <si>
@@ -351,9 +345,6 @@
     <t xml:space="preserve"> Go to end of file</t>
   </si>
   <si>
-    <t>Ctrl+↑ / ↓</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Scroll line up/down</t>
   </si>
   <si>
@@ -474,9 +465,6 @@
     <t xml:space="preserve"> Navigate editor group history</t>
   </si>
   <si>
-    <t>Alt+ ← / →</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Go back / forward</t>
   </si>
   <si>
@@ -534,9 +522,6 @@
     <t xml:space="preserve"> Insert cursor</t>
   </si>
   <si>
-    <t>Ctrl+Alt+ ↑ / ↓</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Insert cursor above / below</t>
   </si>
   <si>
@@ -570,15 +555,9 @@
     <t xml:space="preserve"> Select all occurrences of current word</t>
   </si>
   <si>
-    <t>Shift+Alt+→</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Expand selection</t>
   </si>
   <si>
-    <t>Shift+Alt+←</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Shrink selection</t>
   </si>
   <si>
@@ -687,9 +666,6 @@
     <t>Ctrl+ 1 / 2 / 3</t>
   </si>
   <si>
-    <t>Ctrl+K Ctrl+ ←/→</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Focus into previous/next editor group</t>
   </si>
   <si>
@@ -699,9 +675,6 @@
     <t xml:space="preserve"> Move editor left/right</t>
   </si>
   <si>
-    <t>Ctrl+K ← / →</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Move active editor group</t>
   </si>
   <si>
@@ -987,7 +960,34 @@
     <t>grade2</t>
   </si>
   <si>
-    <t>Ctrl+ &amp;#9650; / &amp;#9660;</t>
+    <t>Ctrl+K left / right</t>
+  </si>
+  <si>
+    <t>Ctrl+K Ctrl+ left / right</t>
+  </si>
+  <si>
+    <t>Ctrl+Alt+ up / down</t>
+  </si>
+  <si>
+    <t>Shift+Alt+ right</t>
+  </si>
+  <si>
+    <t>Shift+Alt+ left</t>
+  </si>
+  <si>
+    <t>Ctrl+ up / down;</t>
+  </si>
+  <si>
+    <t>Alt+ left / right</t>
+  </si>
+  <si>
+    <t>Ctrl+ up / down</t>
+  </si>
+  <si>
+    <t>Shift+Alt + up / down</t>
+  </si>
+  <si>
+    <t>Alt+ up / down</t>
   </si>
 </sst>
 </file>
@@ -1831,11 +1831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A148" sqref="A148"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,13 +1858,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1876,13 +1875,13 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1893,13 +1892,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1910,13 +1909,13 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1927,13 +1926,13 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1944,13 +1943,13 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1961,13 +1960,13 @@
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1978,13 +1977,13 @@
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1995,13 +1994,13 @@
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -2012,13 +2011,13 @@
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -2029,13 +2028,13 @@
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -2046,13 +2045,13 @@
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -2063,13 +2062,13 @@
         <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -2080,13 +2079,13 @@
         <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -2097,13 +2096,13 @@
         <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -2114,13 +2113,13 @@
         <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -2131,13 +2130,13 @@
         <v>42</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -2148,13 +2147,13 @@
         <v>42</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -2165,13 +2164,13 @@
         <v>42</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
@@ -2182,13 +2181,13 @@
         <v>42</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -2199,13 +2198,13 @@
         <v>56</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>48</v>
       </c>
@@ -2216,13 +2215,13 @@
         <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -2233,13 +2232,13 @@
         <v>56</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -2250,13 +2249,13 @@
         <v>56</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -2267,13 +2266,13 @@
         <v>56</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -2284,13 +2283,13 @@
         <v>64</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
@@ -2301,13 +2300,13 @@
         <v>64</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
@@ -2318,13 +2317,13 @@
         <v>64</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -2335,7 +2334,7 @@
         <v>64</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>9</v>
@@ -2352,7 +2351,7 @@
         <v>66</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>67</v>
@@ -2369,7 +2368,7 @@
         <v>66</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>67</v>
@@ -2386,7 +2385,7 @@
         <v>66</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>67</v>
@@ -2403,7 +2402,7 @@
         <v>66</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>67</v>
@@ -2420,7 +2419,7 @@
         <v>66</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>67</v>
@@ -2437,7 +2436,7 @@
         <v>66</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>67</v>
@@ -2454,7 +2453,7 @@
         <v>80</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>67</v>
@@ -2471,7 +2470,7 @@
         <v>80</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>67</v>
@@ -2479,16 +2478,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>67</v>
@@ -2496,16 +2495,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>88</v>
+        <v>316</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>67</v>
@@ -2513,16 +2512,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>67</v>
@@ -2530,16 +2529,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>67</v>
@@ -2547,16 +2546,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>67</v>
@@ -2564,16 +2563,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>67</v>
@@ -2581,7 +2580,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>81</v>
@@ -2590,7 +2589,7 @@
         <v>80</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>67</v>
@@ -2598,16 +2597,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>67</v>
@@ -2615,16 +2614,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>67</v>
@@ -2632,16 +2631,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>67</v>
@@ -2649,16 +2648,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>105</v>
+        <v>315</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>67</v>
@@ -2666,16 +2665,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>67</v>
@@ -2683,16 +2682,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>67</v>
@@ -2700,16 +2699,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>67</v>
@@ -2717,16 +2716,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>67</v>
@@ -2734,16 +2733,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>67</v>
@@ -2751,16 +2750,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>67</v>
@@ -2768,16 +2767,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>67</v>
@@ -2785,16 +2784,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>67</v>
@@ -2802,16 +2801,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>67</v>
@@ -2819,16 +2818,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>67</v>
@@ -2836,16 +2835,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>67</v>
@@ -2853,16 +2852,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>67</v>
@@ -2870,16 +2869,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>67</v>
@@ -2887,16 +2886,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>67</v>
@@ -2907,13 +2906,13 @@
         <v>74</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>67</v>
@@ -2921,16 +2920,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>67</v>
@@ -2938,16 +2937,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>67</v>
@@ -2955,16 +2954,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>67</v>
@@ -2972,16 +2971,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>67</v>
@@ -2989,16 +2988,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>67</v>
@@ -3006,16 +3005,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>146</v>
+        <v>314</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>67</v>
@@ -3023,16 +3022,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>67</v>
@@ -3040,16 +3039,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>67</v>
@@ -3057,16 +3056,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>67</v>
@@ -3074,16 +3073,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>67</v>
@@ -3091,16 +3090,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>67</v>
@@ -3108,16 +3107,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>67</v>
@@ -3125,16 +3124,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>67</v>
@@ -3142,16 +3141,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>67</v>
@@ -3159,16 +3158,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>67</v>
@@ -3176,16 +3175,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>166</v>
+        <v>310</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>67</v>
@@ -3193,16 +3192,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>67</v>
@@ -3210,16 +3209,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>67</v>
@@ -3227,16 +3226,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>67</v>
@@ -3244,16 +3243,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>67</v>
@@ -3261,16 +3260,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>67</v>
@@ -3278,16 +3277,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>178</v>
+        <v>311</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>67</v>
@@ -3295,16 +3294,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>180</v>
+        <v>312</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>67</v>
@@ -3312,16 +3311,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>67</v>
@@ -3329,16 +3328,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>67</v>
@@ -3346,16 +3345,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>67</v>
@@ -3363,16 +3362,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>67</v>
@@ -3380,16 +3379,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>67</v>
@@ -3397,16 +3396,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>67</v>
@@ -3414,16 +3413,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>67</v>
@@ -3431,16 +3430,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>67</v>
@@ -3448,16 +3447,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>67</v>
@@ -3465,16 +3464,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>67</v>
@@ -3482,16 +3481,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>67</v>
@@ -3499,16 +3498,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>67</v>
@@ -3516,16 +3515,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>67</v>
@@ -3533,16 +3532,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>67</v>
@@ -3550,16 +3549,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>67</v>
@@ -3567,16 +3566,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>67</v>
@@ -3584,16 +3583,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>67</v>
@@ -3601,16 +3600,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>67</v>
@@ -3618,16 +3617,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>67</v>
@@ -3635,16 +3634,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>217</v>
+        <v>309</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>67</v>
@@ -3652,16 +3651,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>67</v>
@@ -3669,16 +3668,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>221</v>
+        <v>308</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>67</v>
@@ -3686,16 +3685,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>67</v>
@@ -3703,16 +3702,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>67</v>
@@ -3720,16 +3719,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>67</v>
@@ -3737,16 +3736,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>67</v>
@@ -3754,16 +3753,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>67</v>
@@ -3771,16 +3770,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>67</v>
@@ -3788,16 +3787,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>67</v>
@@ -3805,16 +3804,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>67</v>
@@ -3822,16 +3821,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>67</v>
@@ -3839,16 +3838,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>67</v>
@@ -3856,16 +3855,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>67</v>
@@ -3873,16 +3872,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>67</v>
@@ -3890,16 +3889,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>67</v>
@@ -3907,16 +3906,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>67</v>
@@ -3924,16 +3923,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>67</v>
@@ -3941,16 +3940,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>67</v>
@@ -3958,16 +3957,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>67</v>
@@ -3975,16 +3974,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>67</v>
@@ -3992,16 +3991,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>67</v>
@@ -4009,16 +4008,16 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>67</v>
@@ -4026,16 +4025,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>67</v>
@@ -4043,16 +4042,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>67</v>
@@ -4060,16 +4059,16 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>67</v>
@@ -4077,16 +4076,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>67</v>
@@ -4094,16 +4093,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>67</v>
@@ -4111,16 +4110,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>67</v>
@@ -4128,16 +4127,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>67</v>
@@ -4145,16 +4144,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>67</v>
@@ -4162,16 +4161,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>67</v>
@@ -4179,16 +4178,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>67</v>
@@ -4196,16 +4195,16 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>67</v>
@@ -4213,16 +4212,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>67</v>
@@ -4230,16 +4229,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>67</v>
@@ -4247,16 +4246,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>67</v>
@@ -4264,16 +4263,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>67</v>
@@ -4281,16 +4280,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>67</v>
@@ -4298,16 +4297,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>67</v>
@@ -4318,13 +4317,13 @@
         <v>84</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>67</v>
@@ -4332,16 +4331,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>67</v>
@@ -4349,16 +4348,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>67</v>
@@ -4366,16 +4365,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>67</v>
@@ -4383,29 +4382,23 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E150" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Visual Studio Code for Windows"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E150" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
arrumando problema de compatibilidade do csv
</commit_message>
<xml_diff>
--- a/_data/store-data.xlsx
+++ b/_data/store-data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Desktop\ProjetoCheatSheets\cheatsheets\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B140DE-4C6C-49D8-89BD-3E3A653DB88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC8D19B-4D57-477F-97E2-95ADD8A57AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="360" windowWidth="27615" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="store-data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'store-data'!$A$1:$E$150</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'store-data'!$A$1:$D$150</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="314">
   <si>
     <t>comandos</t>
   </si>
@@ -951,15 +951,6 @@
     <t>INTEGRATED TERMINAL</t>
   </si>
   <si>
-    <t>grade</t>
-  </si>
-  <si>
-    <t>grade1</t>
-  </si>
-  <si>
-    <t>grade2</t>
-  </si>
-  <si>
     <t>Ctrl+K left / right</t>
   </si>
   <si>
@@ -973,9 +964,6 @@
   </si>
   <si>
     <t>Shift+Alt+ left</t>
-  </si>
-  <si>
-    <t>Ctrl+ up / down;</t>
   </si>
   <si>
     <t>Alt+ left / right</t>
@@ -1831,10 +1819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:D150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,12 +1830,11 @@
     <col min="1" max="1" width="31.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="45" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="27.5703125" style="1"/>
+    <col min="4" max="4" width="38.5703125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="27.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1858,13 +1845,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1875,13 +1859,10 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1892,13 +1873,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1909,13 +1887,10 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1926,13 +1901,10 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1943,13 +1915,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1960,13 +1929,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1977,13 +1943,10 @@
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1994,13 +1957,10 @@
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -2011,13 +1971,10 @@
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -2028,13 +1985,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -2045,13 +1999,10 @@
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -2062,13 +2013,10 @@
         <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -2079,13 +2027,10 @@
         <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -2096,13 +2041,10 @@
         <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -2113,13 +2055,10 @@
         <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -2130,13 +2069,10 @@
         <v>42</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -2147,13 +2083,10 @@
         <v>42</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E18" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -2164,13 +2097,10 @@
         <v>42</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E19" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
@@ -2181,13 +2111,10 @@
         <v>42</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E20" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -2198,13 +2125,10 @@
         <v>56</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>48</v>
       </c>
@@ -2215,13 +2139,10 @@
         <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -2232,13 +2153,10 @@
         <v>56</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -2249,13 +2167,10 @@
         <v>56</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -2266,13 +2181,10 @@
         <v>56</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -2283,13 +2195,10 @@
         <v>64</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E26" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
@@ -2300,13 +2209,10 @@
         <v>64</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E27" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
@@ -2317,13 +2223,10 @@
         <v>64</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E28" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -2334,13 +2237,10 @@
         <v>64</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>73</v>
       </c>
@@ -2351,13 +2251,10 @@
         <v>66</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
@@ -2368,13 +2265,10 @@
         <v>66</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>75</v>
       </c>
@@ -2385,13 +2279,10 @@
         <v>66</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
@@ -2402,13 +2293,10 @@
         <v>66</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
@@ -2419,13 +2307,10 @@
         <v>66</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
@@ -2436,13 +2321,10 @@
         <v>66</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
@@ -2453,13 +2335,10 @@
         <v>80</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>84</v>
       </c>
@@ -2470,15 +2349,12 @@
         <v>80</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>86</v>
@@ -2487,15 +2363,12 @@
         <v>80</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>87</v>
@@ -2504,13 +2377,10 @@
         <v>80</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>88</v>
       </c>
@@ -2521,13 +2391,10 @@
         <v>80</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
@@ -2538,13 +2405,10 @@
         <v>80</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>92</v>
       </c>
@@ -2555,13 +2419,10 @@
         <v>80</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>94</v>
       </c>
@@ -2572,13 +2433,10 @@
         <v>80</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>96</v>
       </c>
@@ -2589,13 +2447,10 @@
         <v>80</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>97</v>
       </c>
@@ -2606,13 +2461,10 @@
         <v>80</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>99</v>
       </c>
@@ -2623,13 +2475,10 @@
         <v>80</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>101</v>
       </c>
@@ -2640,15 +2489,12 @@
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>103</v>
@@ -2657,13 +2503,10 @@
         <v>80</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>104</v>
       </c>
@@ -2674,13 +2517,10 @@
         <v>80</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>106</v>
       </c>
@@ -2691,13 +2531,10 @@
         <v>80</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>108</v>
       </c>
@@ -2708,13 +2545,10 @@
         <v>80</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>110</v>
       </c>
@@ -2725,13 +2559,10 @@
         <v>80</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>112</v>
       </c>
@@ -2742,13 +2573,10 @@
         <v>80</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>114</v>
       </c>
@@ -2759,13 +2587,10 @@
         <v>80</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>116</v>
       </c>
@@ -2776,13 +2601,10 @@
         <v>80</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>118</v>
       </c>
@@ -2793,13 +2615,10 @@
         <v>80</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>120</v>
       </c>
@@ -2810,13 +2629,10 @@
         <v>80</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>122</v>
       </c>
@@ -2827,13 +2643,10 @@
         <v>80</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>124</v>
       </c>
@@ -2844,13 +2657,10 @@
         <v>80</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>126</v>
       </c>
@@ -2861,13 +2671,10 @@
         <v>80</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>128</v>
       </c>
@@ -2878,13 +2685,10 @@
         <v>296</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>130</v>
       </c>
@@ -2895,13 +2699,10 @@
         <v>296</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>74</v>
       </c>
@@ -2912,13 +2713,10 @@
         <v>296</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>133</v>
       </c>
@@ -2929,13 +2727,10 @@
         <v>296</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>135</v>
       </c>
@@ -2946,13 +2741,10 @@
         <v>296</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>137</v>
       </c>
@@ -2963,13 +2755,10 @@
         <v>296</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>139</v>
       </c>
@@ -2980,13 +2769,10 @@
         <v>296</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>141</v>
       </c>
@@ -2997,15 +2783,12 @@
         <v>296</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>143</v>
@@ -3014,13 +2797,10 @@
         <v>296</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>144</v>
       </c>
@@ -3031,13 +2811,10 @@
         <v>296</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>146</v>
       </c>
@@ -3048,13 +2825,10 @@
         <v>297</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>148</v>
       </c>
@@ -3065,13 +2839,10 @@
         <v>297</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>150</v>
       </c>
@@ -3082,13 +2853,10 @@
         <v>297</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>152</v>
       </c>
@@ -3099,13 +2867,10 @@
         <v>297</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>154</v>
       </c>
@@ -3116,13 +2881,10 @@
         <v>297</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>156</v>
       </c>
@@ -3133,13 +2895,10 @@
         <v>297</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>158</v>
       </c>
@@ -3150,13 +2909,10 @@
         <v>297</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>160</v>
       </c>
@@ -3167,15 +2923,12 @@
         <v>298</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>162</v>
@@ -3184,13 +2937,10 @@
         <v>298</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>163</v>
       </c>
@@ -3201,13 +2951,10 @@
         <v>298</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>165</v>
       </c>
@@ -3218,13 +2965,10 @@
         <v>298</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>167</v>
       </c>
@@ -3235,13 +2979,10 @@
         <v>298</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>169</v>
       </c>
@@ -3252,13 +2993,10 @@
         <v>298</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>171</v>
       </c>
@@ -3269,15 +3007,12 @@
         <v>298</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>173</v>
@@ -3286,15 +3021,12 @@
         <v>298</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>174</v>
@@ -3303,13 +3035,10 @@
         <v>298</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>175</v>
       </c>
@@ -3320,13 +3049,10 @@
         <v>298</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>177</v>
       </c>
@@ -3337,13 +3063,10 @@
         <v>298</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>178</v>
       </c>
@@ -3354,13 +3077,10 @@
         <v>298</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>293</v>
       </c>
@@ -3371,13 +3091,10 @@
         <v>299</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>181</v>
       </c>
@@ -3388,13 +3105,10 @@
         <v>299</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>183</v>
       </c>
@@ -3405,13 +3119,10 @@
         <v>299</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>185</v>
       </c>
@@ -3422,13 +3133,10 @@
         <v>299</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>187</v>
       </c>
@@ -3439,13 +3147,10 @@
         <v>299</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>189</v>
       </c>
@@ -3456,13 +3161,10 @@
         <v>299</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>191</v>
       </c>
@@ -3473,13 +3175,10 @@
         <v>299</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>193</v>
       </c>
@@ -3490,13 +3189,10 @@
         <v>299</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>195</v>
       </c>
@@ -3507,13 +3203,10 @@
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>197</v>
       </c>
@@ -3524,13 +3217,10 @@
         <v>299</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>199</v>
       </c>
@@ -3541,13 +3231,10 @@
         <v>299</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>201</v>
       </c>
@@ -3558,13 +3245,10 @@
         <v>299</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>294</v>
       </c>
@@ -3575,13 +3259,10 @@
         <v>300</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>205</v>
       </c>
@@ -3592,13 +3273,10 @@
         <v>300</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>207</v>
       </c>
@@ -3609,13 +3287,10 @@
         <v>300</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>209</v>
       </c>
@@ -3626,15 +3301,12 @@
         <v>300</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>210</v>
@@ -3643,13 +3315,10 @@
         <v>300</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>211</v>
       </c>
@@ -3660,15 +3329,12 @@
         <v>300</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>213</v>
@@ -3677,13 +3343,10 @@
         <v>300</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>214</v>
       </c>
@@ -3694,13 +3357,10 @@
         <v>301</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>216</v>
       </c>
@@ -3711,13 +3371,10 @@
         <v>301</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>218</v>
       </c>
@@ -3728,13 +3385,10 @@
         <v>301</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>220</v>
       </c>
@@ -3745,13 +3399,10 @@
         <v>301</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>222</v>
       </c>
@@ -3762,13 +3413,10 @@
         <v>301</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>203</v>
       </c>
@@ -3779,13 +3427,10 @@
         <v>301</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>225</v>
       </c>
@@ -3796,13 +3441,10 @@
         <v>301</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>227</v>
       </c>
@@ -3813,13 +3455,10 @@
         <v>301</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>229</v>
       </c>
@@ -3830,13 +3469,10 @@
         <v>301</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>231</v>
       </c>
@@ -3847,13 +3483,10 @@
         <v>301</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>141</v>
       </c>
@@ -3864,13 +3497,10 @@
         <v>301</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>234</v>
       </c>
@@ -3881,13 +3511,10 @@
         <v>301</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>236</v>
       </c>
@@ -3898,13 +3525,10 @@
         <v>301</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>238</v>
       </c>
@@ -3915,13 +3539,10 @@
         <v>301</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>240</v>
       </c>
@@ -3932,13 +3553,10 @@
         <v>302</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>242</v>
       </c>
@@ -3949,13 +3567,10 @@
         <v>302</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>244</v>
       </c>
@@ -3966,13 +3581,10 @@
         <v>302</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>246</v>
       </c>
@@ -3983,13 +3595,10 @@
         <v>302</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>248</v>
       </c>
@@ -4000,13 +3609,10 @@
         <v>302</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>250</v>
       </c>
@@ -4017,13 +3623,10 @@
         <v>302</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>252</v>
       </c>
@@ -4034,13 +3637,10 @@
         <v>302</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>254</v>
       </c>
@@ -4051,13 +3651,10 @@
         <v>302</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>256</v>
       </c>
@@ -4068,13 +3665,10 @@
         <v>302</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>258</v>
       </c>
@@ -4085,13 +3679,10 @@
         <v>302</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>260</v>
       </c>
@@ -4102,13 +3693,10 @@
         <v>302</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>262</v>
       </c>
@@ -4119,13 +3707,10 @@
         <v>302</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>264</v>
       </c>
@@ -4136,13 +3721,10 @@
         <v>302</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>266</v>
       </c>
@@ -4153,13 +3735,10 @@
         <v>302</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>268</v>
       </c>
@@ -4170,13 +3749,10 @@
         <v>302</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>270</v>
       </c>
@@ -4187,13 +3763,10 @@
         <v>303</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>272</v>
       </c>
@@ -4204,13 +3777,10 @@
         <v>303</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>274</v>
       </c>
@@ -4221,13 +3791,10 @@
         <v>303</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>276</v>
       </c>
@@ -4238,13 +3805,10 @@
         <v>303</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>278</v>
       </c>
@@ -4255,13 +3819,10 @@
         <v>303</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>280</v>
       </c>
@@ -4272,13 +3833,10 @@
         <v>303</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>282</v>
       </c>
@@ -4289,13 +3847,10 @@
         <v>304</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>284</v>
       </c>
@@ -4306,13 +3861,10 @@
         <v>304</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>84</v>
       </c>
@@ -4323,13 +3875,10 @@
         <v>304</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>287</v>
       </c>
@@ -4340,15 +3889,12 @@
         <v>304</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>289</v>
@@ -4357,13 +3903,10 @@
         <v>304</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>290</v>
       </c>
@@ -4374,13 +3917,10 @@
         <v>304</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>291</v>
       </c>
@@ -4391,14 +3931,10 @@
         <v>304</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E150" s="1" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E150" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adicionado pagina e dados para pycharm
</commit_message>
<xml_diff>
--- a/_data/store-data.xlsx
+++ b/_data/store-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Desktop\ProjetoCheatSheets\cheatsheets\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC8D19B-4D57-477F-97E2-95ADD8A57AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2351BB4D-9A53-429F-BBF9-C8A1BC9E1604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8655" yWindow="360" windowWidth="27615" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="store-data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="350">
   <si>
     <t>comandos</t>
   </si>
@@ -976,13 +976,159 @@
   </si>
   <si>
     <t>Alt+ up / down</t>
+  </si>
+  <si>
+    <t>Ctrl+Shift+A</t>
+  </si>
+  <si>
+    <t>Find action by name</t>
+  </si>
+  <si>
+    <t>Double Shift</t>
+  </si>
+  <si>
+    <t>Search Everywhere</t>
+  </si>
+  <si>
+    <t>Show the list of available intention actions</t>
+  </si>
+  <si>
+    <t>Alt+F1</t>
+  </si>
+  <si>
+    <r>
+      <t>Switch between views (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF167DFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF27282C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF167DFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Structure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF27282C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, etc.)</t>
+    </r>
+  </si>
+  <si>
+    <t>Ctrl+Tab</t>
+  </si>
+  <si>
+    <t>Switch between the tool windows and files opened in the editor</t>
+  </si>
+  <si>
+    <t>Alt+Home</t>
+  </si>
+  <si>
+    <t>Show the Navigation bar</t>
+  </si>
+  <si>
+    <t>Ctrl+J</t>
+  </si>
+  <si>
+    <t>Insert a live template</t>
+  </si>
+  <si>
+    <t>Ctrl+Alt+J</t>
+  </si>
+  <si>
+    <t>Surround with a live template</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>Edit an item from the Project or another tree view</t>
+  </si>
+  <si>
+    <t>Ctrl+Slash</t>
+  </si>
+  <si>
+    <t>Ctrl+Shift+Slash</t>
+  </si>
+  <si>
+    <t>Comment or uncomment a line or fragment of code with a line or block comment</t>
+  </si>
+  <si>
+    <t>Find class or file by name</t>
+  </si>
+  <si>
+    <t>Duplicate the current line or selection</t>
+  </si>
+  <si>
+    <t>Ctrl+W and Ctrl+Shift+W</t>
+  </si>
+  <si>
+    <t>Incremental expression selection</t>
+  </si>
+  <si>
+    <t>Find text string in the current file</t>
+  </si>
+  <si>
+    <t>Ctrl+Shift+F</t>
+  </si>
+  <si>
+    <t>Find text in the project or in the specified directory</t>
+  </si>
+  <si>
+    <t>Ctrl+Shift+F7</t>
+  </si>
+  <si>
+    <t>Quickly view the usages of the selected symbol</t>
+  </si>
+  <si>
+    <t>Ctrl+NumPad Plus</t>
+  </si>
+  <si>
+    <t>Ctrl+NumPad –</t>
+  </si>
+  <si>
+    <t>Expand or collapse a code block in the editor</t>
+  </si>
+  <si>
+    <t>Ctrl+Space</t>
+  </si>
+  <si>
+    <t>Invoke code completion</t>
+  </si>
+  <si>
+    <t>Pycharm</t>
+  </si>
+  <si>
+    <t>EDITING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1116,6 +1262,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF27282C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF167DFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1459,11 +1617,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1819,2119 +1974,2412 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="27.5703125" style="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>64</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>313</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>312</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>80</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>98</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>99</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>80</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>101</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>80</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>311</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>104</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>80</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>80</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>109</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" t="s">
         <v>80</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>111</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>80</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>112</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>113</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>115</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>80</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>116</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>117</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>80</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>119</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" t="s">
         <v>80</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" t="s">
         <v>80</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>122</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>123</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" t="s">
         <v>80</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" t="s">
         <v>80</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="A60" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>127</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" t="s">
         <v>80</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>129</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" t="s">
         <v>296</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>131</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" t="s">
         <v>296</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>74</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>132</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" t="s">
         <v>296</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>133</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>134</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" t="s">
         <v>296</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>135</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>136</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" t="s">
         <v>296</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>137</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" t="s">
         <v>296</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
         <v>139</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>140</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" t="s">
         <v>296</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="A68" t="s">
         <v>141</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>142</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" t="s">
         <v>296</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="A69" t="s">
         <v>310</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>143</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" t="s">
         <v>296</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>144</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>145</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" t="s">
         <v>296</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="A71" t="s">
         <v>146</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>147</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" t="s">
         <v>297</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>148</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>149</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" t="s">
         <v>297</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>150</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>151</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" t="s">
         <v>297</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>152</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" t="s">
         <v>153</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" t="s">
         <v>297</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="A75" t="s">
         <v>154</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>155</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" t="s">
         <v>297</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>156</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" t="s">
         <v>157</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" t="s">
         <v>297</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="A77" t="s">
         <v>158</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" t="s">
         <v>159</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" t="s">
         <v>297</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+      <c r="A78" t="s">
         <v>160</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" t="s">
         <v>161</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" t="s">
         <v>298</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="A79" t="s">
         <v>307</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" t="s">
         <v>162</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" t="s">
         <v>298</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="A80" t="s">
         <v>163</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" t="s">
         <v>164</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" t="s">
         <v>298</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="A81" t="s">
         <v>165</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" t="s">
         <v>166</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" t="s">
         <v>298</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="A82" t="s">
         <v>167</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" t="s">
         <v>168</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" t="s">
         <v>298</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="A83" t="s">
         <v>169</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" t="s">
         <v>170</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" t="s">
         <v>298</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="A84" t="s">
         <v>171</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" t="s">
         <v>172</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" t="s">
         <v>298</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="A85" t="s">
         <v>308</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" t="s">
         <v>173</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" t="s">
         <v>298</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D85" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="A86" t="s">
         <v>309</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" t="s">
         <v>174</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" t="s">
         <v>298</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="A87" t="s">
         <v>175</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" t="s">
         <v>176</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" t="s">
         <v>298</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D87" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="A88" t="s">
         <v>177</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" t="s">
         <v>176</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" t="s">
         <v>298</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="A89" t="s">
         <v>178</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" t="s">
         <v>179</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" t="s">
         <v>298</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="A90" t="s">
         <v>293</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" t="s">
         <v>180</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" t="s">
         <v>299</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="A91" t="s">
         <v>181</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" t="s">
         <v>182</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" t="s">
         <v>299</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="A92" t="s">
         <v>183</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" t="s">
         <v>184</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" t="s">
         <v>299</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="A93" t="s">
         <v>185</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" t="s">
         <v>186</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" t="s">
         <v>299</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="A94" t="s">
         <v>187</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" t="s">
         <v>188</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" t="s">
         <v>299</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="A95" t="s">
         <v>189</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" t="s">
         <v>190</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" t="s">
         <v>299</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="A96" t="s">
         <v>191</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" t="s">
         <v>192</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" t="s">
         <v>299</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="A97" t="s">
         <v>193</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" t="s">
         <v>194</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" t="s">
         <v>299</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D97" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="A98" t="s">
         <v>195</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" t="s">
         <v>196</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" t="s">
         <v>299</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D98" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="A99" t="s">
         <v>197</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" t="s">
         <v>198</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" t="s">
         <v>299</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="A100" t="s">
         <v>199</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" t="s">
         <v>200</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" t="s">
         <v>299</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="A101" t="s">
         <v>201</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" t="s">
         <v>202</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" t="s">
         <v>299</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="A102" t="s">
         <v>294</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" t="s">
         <v>204</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" t="s">
         <v>300</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+      <c r="A103" t="s">
         <v>205</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" t="s">
         <v>206</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" t="s">
         <v>300</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="A104" t="s">
         <v>207</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" t="s">
         <v>208</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" t="s">
         <v>300</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="A105" t="s">
         <v>209</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" t="s">
         <v>295</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" t="s">
         <v>300</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+      <c r="A106" t="s">
         <v>306</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" t="s">
         <v>210</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" t="s">
         <v>300</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D106" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="A107" t="s">
         <v>211</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" t="s">
         <v>212</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" t="s">
         <v>300</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D107" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="A108" t="s">
         <v>305</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" t="s">
         <v>213</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" t="s">
         <v>300</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D108" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="A109" t="s">
         <v>214</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" t="s">
         <v>215</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" t="s">
         <v>301</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D109" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="A110" t="s">
         <v>216</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" t="s">
         <v>217</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" t="s">
         <v>301</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D110" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="A111" t="s">
         <v>218</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" t="s">
         <v>219</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" t="s">
         <v>301</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D111" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="A112" t="s">
         <v>220</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" t="s">
         <v>221</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" t="s">
         <v>301</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D112" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="A113" t="s">
         <v>222</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" t="s">
         <v>223</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" t="s">
         <v>301</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D113" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+      <c r="A114" t="s">
         <v>203</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" t="s">
         <v>224</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" t="s">
         <v>301</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D114" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+      <c r="A115" t="s">
         <v>225</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" t="s">
         <v>226</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" t="s">
         <v>301</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D115" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="A116" t="s">
         <v>227</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" t="s">
         <v>228</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" t="s">
         <v>301</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D116" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+      <c r="A117" t="s">
         <v>229</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" t="s">
         <v>230</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" t="s">
         <v>301</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D117" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="A118" t="s">
         <v>231</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" t="s">
         <v>232</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" t="s">
         <v>301</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D118" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+      <c r="A119" t="s">
         <v>141</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" t="s">
         <v>233</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" t="s">
         <v>301</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D119" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="A120" t="s">
         <v>234</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" t="s">
         <v>235</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" t="s">
         <v>301</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D120" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="A121" t="s">
         <v>236</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" t="s">
         <v>237</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" t="s">
         <v>301</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D121" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+      <c r="A122" t="s">
         <v>238</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" t="s">
         <v>239</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" t="s">
         <v>301</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D122" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+      <c r="A123" t="s">
         <v>240</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" t="s">
         <v>241</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" t="s">
         <v>302</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D123" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+      <c r="A124" t="s">
         <v>242</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" t="s">
         <v>243</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C124" t="s">
         <v>302</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D124" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+      <c r="A125" t="s">
         <v>244</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" t="s">
         <v>245</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" t="s">
         <v>302</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D125" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+      <c r="A126" t="s">
         <v>246</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" t="s">
         <v>247</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" t="s">
         <v>302</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="D126" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="A127" t="s">
         <v>248</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" t="s">
         <v>249</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" t="s">
         <v>302</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="D127" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+      <c r="A128" t="s">
         <v>250</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" t="s">
         <v>251</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C128" t="s">
         <v>302</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="D128" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+      <c r="A129" t="s">
         <v>252</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" t="s">
         <v>253</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" t="s">
         <v>302</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="D129" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+      <c r="A130" t="s">
         <v>254</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B130" t="s">
         <v>255</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C130" t="s">
         <v>302</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="D130" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+      <c r="A131" t="s">
         <v>256</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" t="s">
         <v>257</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C131" t="s">
         <v>302</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="D131" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="A132" t="s">
         <v>258</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" t="s">
         <v>259</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="C132" t="s">
         <v>302</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="D132" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+      <c r="A133" t="s">
         <v>260</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" t="s">
         <v>261</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C133" t="s">
         <v>302</v>
       </c>
-      <c r="D133" s="1" t="s">
+      <c r="D133" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
+      <c r="A134" t="s">
         <v>262</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" t="s">
         <v>263</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C134" t="s">
         <v>302</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="D134" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+      <c r="A135" t="s">
         <v>264</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" t="s">
         <v>265</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C135" t="s">
         <v>302</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="D135" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
+      <c r="A136" t="s">
         <v>266</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" t="s">
         <v>267</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C136" t="s">
         <v>302</v>
       </c>
-      <c r="D136" s="1" t="s">
+      <c r="D136" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+      <c r="A137" t="s">
         <v>268</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" t="s">
         <v>269</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C137" t="s">
         <v>302</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="D137" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+      <c r="A138" t="s">
         <v>270</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" t="s">
         <v>271</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="C138" t="s">
         <v>303</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="D138" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
+      <c r="A139" t="s">
         <v>272</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" t="s">
         <v>273</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C139" t="s">
         <v>303</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="D139" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
+      <c r="A140" t="s">
         <v>274</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" t="s">
         <v>275</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="C140" t="s">
         <v>303</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="D140" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
+      <c r="A141" t="s">
         <v>276</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" t="s">
         <v>277</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C141" t="s">
         <v>303</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="D141" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
+      <c r="A142" t="s">
         <v>278</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" t="s">
         <v>279</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C142" t="s">
         <v>303</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="D142" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
+      <c r="A143" t="s">
         <v>280</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" t="s">
         <v>281</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C143" t="s">
         <v>303</v>
       </c>
-      <c r="D143" s="1" t="s">
+      <c r="D143" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
+      <c r="A144" t="s">
         <v>282</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" t="s">
         <v>283</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="C144" t="s">
         <v>304</v>
       </c>
-      <c r="D144" s="1" t="s">
+      <c r="D144" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
+      <c r="A145" t="s">
         <v>284</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B145" t="s">
         <v>285</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C145" t="s">
         <v>304</v>
       </c>
-      <c r="D145" s="1" t="s">
+      <c r="D145" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
+      <c r="A146" t="s">
         <v>84</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B146" t="s">
         <v>286</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C146" t="s">
         <v>304</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="D146" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
+      <c r="A147" t="s">
         <v>287</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B147" t="s">
         <v>288</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C147" t="s">
         <v>304</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="D147" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
+      <c r="A148" t="s">
         <v>311</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B148" t="s">
         <v>289</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C148" t="s">
         <v>304</v>
       </c>
-      <c r="D148" s="1" t="s">
+      <c r="D148" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
+      <c r="A149" t="s">
         <v>290</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B149" t="s">
         <v>105</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C149" t="s">
         <v>304</v>
       </c>
-      <c r="D149" s="1" t="s">
+      <c r="D149" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
+      <c r="A150" t="s">
         <v>291</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B150" t="s">
         <v>292</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="C150" t="s">
         <v>304</v>
       </c>
-      <c r="D150" s="1" t="s">
-        <v>67</v>
+      <c r="D150" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>314</v>
+      </c>
+      <c r="B151" t="s">
+        <v>315</v>
+      </c>
+      <c r="C151" t="s">
+        <v>349</v>
+      </c>
+      <c r="D151" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>316</v>
+      </c>
+      <c r="B152" t="s">
+        <v>317</v>
+      </c>
+      <c r="C152" t="s">
+        <v>349</v>
+      </c>
+      <c r="D152" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>318</v>
+      </c>
+      <c r="C153" t="s">
+        <v>349</v>
+      </c>
+      <c r="D153" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>319</v>
+      </c>
+      <c r="B154" t="s">
+        <v>320</v>
+      </c>
+      <c r="C154" t="s">
+        <v>349</v>
+      </c>
+      <c r="D154" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>321</v>
+      </c>
+      <c r="B155" t="s">
+        <v>322</v>
+      </c>
+      <c r="C155" t="s">
+        <v>349</v>
+      </c>
+      <c r="D155" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>323</v>
+      </c>
+      <c r="B156" t="s">
+        <v>324</v>
+      </c>
+      <c r="C156" t="s">
+        <v>349</v>
+      </c>
+      <c r="D156" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>325</v>
+      </c>
+      <c r="B157" t="s">
+        <v>326</v>
+      </c>
+      <c r="C157" t="s">
+        <v>349</v>
+      </c>
+      <c r="D157" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>327</v>
+      </c>
+      <c r="B158" t="s">
+        <v>328</v>
+      </c>
+      <c r="C158" t="s">
+        <v>349</v>
+      </c>
+      <c r="D158" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>329</v>
+      </c>
+      <c r="B159" t="s">
+        <v>330</v>
+      </c>
+      <c r="C159" t="s">
+        <v>349</v>
+      </c>
+      <c r="D159" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>331</v>
+      </c>
+      <c r="B160" t="s">
+        <v>333</v>
+      </c>
+      <c r="C160" t="s">
+        <v>349</v>
+      </c>
+      <c r="D160" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>332</v>
+      </c>
+      <c r="B161" t="s">
+        <v>333</v>
+      </c>
+      <c r="C161" t="s">
+        <v>349</v>
+      </c>
+      <c r="D161" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>214</v>
+      </c>
+      <c r="B162" t="s">
+        <v>334</v>
+      </c>
+      <c r="C162" t="s">
+        <v>349</v>
+      </c>
+      <c r="D162" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>75</v>
+      </c>
+      <c r="B163" t="s">
+        <v>334</v>
+      </c>
+      <c r="C163" t="s">
+        <v>349</v>
+      </c>
+      <c r="D163" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>154</v>
+      </c>
+      <c r="B164" t="s">
+        <v>335</v>
+      </c>
+      <c r="C164" t="s">
+        <v>349</v>
+      </c>
+      <c r="D164" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>336</v>
+      </c>
+      <c r="B165" t="s">
+        <v>337</v>
+      </c>
+      <c r="C165" t="s">
+        <v>349</v>
+      </c>
+      <c r="D165" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>146</v>
+      </c>
+      <c r="B166" t="s">
+        <v>338</v>
+      </c>
+      <c r="C166" t="s">
+        <v>349</v>
+      </c>
+      <c r="D166" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>339</v>
+      </c>
+      <c r="B167" t="s">
+        <v>340</v>
+      </c>
+      <c r="C167" t="s">
+        <v>349</v>
+      </c>
+      <c r="D167" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>341</v>
+      </c>
+      <c r="B168" t="s">
+        <v>342</v>
+      </c>
+      <c r="C168" t="s">
+        <v>349</v>
+      </c>
+      <c r="D168" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>343</v>
+      </c>
+      <c r="B169" t="s">
+        <v>345</v>
+      </c>
+      <c r="C169" t="s">
+        <v>349</v>
+      </c>
+      <c r="D169" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>344</v>
+      </c>
+      <c r="B170" t="s">
+        <v>345</v>
+      </c>
+      <c r="C170" t="s">
+        <v>349</v>
+      </c>
+      <c r="D170" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>346</v>
+      </c>
+      <c r="B171" t="s">
+        <v>347</v>
+      </c>
+      <c r="C171" t="s">
+        <v>349</v>
+      </c>
+      <c r="D171" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arrumando dados do pycharm
</commit_message>
<xml_diff>
--- a/_data/store-data.xlsx
+++ b/_data/store-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Desktop\ProjetoCheatSheets\cheatsheets\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2351BB4D-9A53-429F-BBF9-C8A1BC9E1604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89697CE7-3CA6-45AA-B517-D056BB655C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8655" yWindow="360" windowWidth="27615" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -990,53 +990,9 @@
     <t>Search Everywhere</t>
   </si>
   <si>
-    <t>Show the list of available intention actions</t>
-  </si>
-  <si>
     <t>Alt+F1</t>
   </si>
   <si>
-    <r>
-      <t>Switch between views (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color rgb="FF167DFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Project</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color rgb="FF27282C"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color rgb="FF167DFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Structure</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color rgb="FF27282C"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, etc.)</t>
-    </r>
-  </si>
-  <si>
     <t>Ctrl+Tab</t>
   </si>
   <si>
@@ -1106,9 +1062,6 @@
     <t>Ctrl+NumPad Plus</t>
   </si>
   <si>
-    <t>Ctrl+NumPad –</t>
-  </si>
-  <si>
     <t>Expand or collapse a code block in the editor</t>
   </si>
   <si>
@@ -1122,13 +1075,22 @@
   </si>
   <si>
     <t>EDITING</t>
+  </si>
+  <si>
+    <t>Ctrl+NumPad Minus</t>
+  </si>
+  <si>
+    <t>Switch between views</t>
+  </si>
+  <si>
+    <t>Show the list of available intention actions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1262,18 +1224,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color rgb="FF27282C"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color rgb="FF167DFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1976,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4096,10 +4046,10 @@
         <v>315</v>
       </c>
       <c r="C151" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D151" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -4110,10 +4060,10 @@
         <v>317</v>
       </c>
       <c r="C152" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D152" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -4121,125 +4071,125 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>318</v>
+        <v>349</v>
       </c>
       <c r="C153" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D153" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B154" t="s">
-        <v>320</v>
+        <v>348</v>
       </c>
       <c r="C154" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D154" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B155" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C155" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D155" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B156" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C156" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D156" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B157" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C157" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D157" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B158" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C158" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D158" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B159" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C159" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D159" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>329</v>
+      </c>
+      <c r="B160" t="s">
         <v>331</v>
       </c>
-      <c r="B160" t="s">
-        <v>333</v>
-      </c>
       <c r="C160" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D160" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B161" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C161" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D161" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4247,13 +4197,13 @@
         <v>214</v>
       </c>
       <c r="B162" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C162" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D162" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4261,13 +4211,13 @@
         <v>75</v>
       </c>
       <c r="B163" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C163" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D163" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4275,27 +4225,27 @@
         <v>154</v>
       </c>
       <c r="B164" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C164" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D164" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B165" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C165" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D165" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4303,83 +4253,83 @@
         <v>146</v>
       </c>
       <c r="B166" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C166" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D166" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B167" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C167" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D167" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B168" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C168" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D168" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B169" t="s">
+        <v>342</v>
+      </c>
+      <c r="C169" t="s">
+        <v>346</v>
+      </c>
+      <c r="D169" t="s">
         <v>345</v>
-      </c>
-      <c r="C169" t="s">
-        <v>349</v>
-      </c>
-      <c r="D169" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B170" t="s">
+        <v>342</v>
+      </c>
+      <c r="C170" t="s">
+        <v>346</v>
+      </c>
+      <c r="D170" t="s">
         <v>345</v>
-      </c>
-      <c r="C170" t="s">
-        <v>349</v>
-      </c>
-      <c r="D170" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>343</v>
+      </c>
+      <c r="B171" t="s">
+        <v>344</v>
+      </c>
+      <c r="C171" t="s">
         <v>346</v>
       </c>
-      <c r="B171" t="s">
-        <v>347</v>
-      </c>
-      <c r="C171" t="s">
-        <v>349</v>
-      </c>
       <c r="D171" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>